<commit_message>
"Enhanced the automation framework"
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Guru99BankTestData.xlsx
+++ b/src/test/resources/testData/Guru99BankTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Password</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>expectedMessage</t>
-  </si>
-  <si>
-    <t>User-ID must not be blank</t>
   </si>
   <si>
     <t>User or Password is not valid</t>
@@ -421,7 +418,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -447,19 +444,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -469,28 +466,28 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -501,10 +498,10 @@
     <row r="4" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -514,13 +511,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>

</xml_diff>

<commit_message>
Added testcases for manager page
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Guru99BankTestData.xlsx
+++ b/src/test/resources/testData/Guru99BankTestData.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\selenium\Pom\PageObjectModel-master\Guru99BankAutomationF\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A67B2AC4-F97C-4695-BF0D-67F060FE225D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="132" windowWidth="22932" windowHeight="9240"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="ManagerPage" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Password</t>
   </si>
@@ -60,13 +66,73 @@
   </si>
   <si>
     <t xml:space="preserve"> Guru99 Bank Home Page </t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>New Customer</t>
+  </si>
+  <si>
+    <t>Edit Customer</t>
+  </si>
+  <si>
+    <t>Delete Customer</t>
+  </si>
+  <si>
+    <t>New Account</t>
+  </si>
+  <si>
+    <t>Edit Account</t>
+  </si>
+  <si>
+    <t>Delete Account</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Withdrawal</t>
+  </si>
+  <si>
+    <t>Fund Transfer</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>Balance Enquiry</t>
+  </si>
+  <si>
+    <t>Mini Statement</t>
+  </si>
+  <si>
+    <t>Customised Statement</t>
+  </si>
+  <si>
+    <t>Log out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menuOptions </t>
+  </si>
+  <si>
+    <t>welcomeMessage</t>
+  </si>
+  <si>
+    <t>managerIdMessage</t>
+  </si>
+  <si>
+    <t>Welcome To Manager's Page of Guru99 Bank</t>
+  </si>
+  <si>
+    <t>Manger Id : %s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +151,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,13 +192,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -173,7 +253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -205,9 +285,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,6 +337,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -414,14 +530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.21875" customWidth="1"/>
@@ -433,7 +549,7 @@
     <col min="8" max="8" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -459,7 +575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -477,11 +593,11 @@
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -495,7 +611,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -509,7 +625,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -531,13 +647,142 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="40.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NewCustomer Page Automation Testcases added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Guru99BankTestData.xlsx
+++ b/src/test/resources/testData/Guru99BankTestData.xlsx
@@ -8,20 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\selenium\Pom\PageObjectModel-master\Guru99BankAutomationF\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A67B2AC4-F97C-4695-BF0D-67F060FE225D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F63EE6-5420-4B0E-B5A9-29EA4C05CF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-144" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="2" r:id="rId1"/>
     <sheet name="ManagerPage" sheetId="3" r:id="rId2"/>
+    <sheet name="NewCustomerPage" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
   <si>
     <t>Password</t>
   </si>
@@ -126,13 +138,178 @@
   </si>
   <si>
     <t>Manger Id : %s</t>
+  </si>
+  <si>
+    <t>HeadingMessage</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>CustomerNameField</t>
+  </si>
+  <si>
+    <t>CustomerNameExpectedMessage</t>
+  </si>
+  <si>
+    <t>DateOfBirthField</t>
+  </si>
+  <si>
+    <t>DateOfBirthExpectedMessage</t>
+  </si>
+  <si>
+    <t>CityField</t>
+  </si>
+  <si>
+    <t>CItyFieldExpectedMessage</t>
+  </si>
+  <si>
+    <t>StateField</t>
+  </si>
+  <si>
+    <t>StateFieldExpectedMessage</t>
+  </si>
+  <si>
+    <t>PinCodeField</t>
+  </si>
+  <si>
+    <t>PinCodeExpectedMessage</t>
+  </si>
+  <si>
+    <t>MobileNumberField</t>
+  </si>
+  <si>
+    <t>MobileNumberExpectedMessage</t>
+  </si>
+  <si>
+    <t>EmailField</t>
+  </si>
+  <si>
+    <t>EmailExpectedMessage</t>
+  </si>
+  <si>
+    <t>PasswordField</t>
+  </si>
+  <si>
+    <t>PasswordExpectedMessage</t>
+  </si>
+  <si>
+    <t>Add New Customer</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>!@#$%^*&amp;*^)</t>
+  </si>
+  <si>
+    <t>Customer name must not be blank</t>
+  </si>
+  <si>
+    <t>First character can not have space</t>
+  </si>
+  <si>
+    <t>Special characters are not allowed</t>
+  </si>
+  <si>
+    <t>Numbers are not allowed</t>
+  </si>
+  <si>
+    <t>Date Field must not be blank</t>
+  </si>
+  <si>
+    <t>!@#$$%</t>
+  </si>
+  <si>
+    <t>City Field must not be blank</t>
+  </si>
+  <si>
+    <t>PIN Code must not be blank</t>
+  </si>
+  <si>
+    <t>PIN Code must have 6 Digits</t>
+  </si>
+  <si>
+    <t>12 234</t>
+  </si>
+  <si>
+    <t>Characters are not allowed</t>
+  </si>
+  <si>
+    <t>123 2344</t>
+  </si>
+  <si>
+    <t>Email-ID must not be blank</t>
+  </si>
+  <si>
+    <t>!@#$</t>
+  </si>
+  <si>
+    <t>Email-ID is not valid</t>
+  </si>
+  <si>
+    <t>Password must not be blank</t>
+  </si>
+  <si>
+    <t>Address Field must not be blank</t>
+  </si>
+  <si>
+    <t>FieldsLabel</t>
+  </si>
+  <si>
+    <t>AddressField</t>
+  </si>
+  <si>
+    <t>AddressExpectedMessage</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Mobile no must not be blank</t>
+  </si>
+  <si>
+    <t>State must not be blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,8 +317,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +342,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,16 +376,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -537,19 +745,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="6" max="6" width="38.44140625" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -575,7 +783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -597,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -611,7 +819,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -625,7 +833,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -650,18 +858,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
@@ -672,7 +880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -683,98 +891,98 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -785,4 +993,481 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC305B47-AD8C-4FCA-A0E3-8E1F41D4C59C}">
+  <dimension ref="A1:U11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="7" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
+        <v>123456</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="4">
+        <v>123456</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1234</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{4B8C438E-8AAB-4561-B422-21F58C8B478C}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{2EB559C8-61E3-4587-9382-8776EAAA095F}"/>
+    <hyperlink ref="J5" r:id="rId3" xr:uid="{738532B5-0DBF-4CA5-B160-5425DEDF6DD5}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{91C37AA5-3114-4AF3-9C31-F3B7E7A4BF7A}"/>
+    <hyperlink ref="N5" r:id="rId5" xr:uid="{E464460E-95EC-46F7-8E80-9441CB6847BC}"/>
+    <hyperlink ref="P5" r:id="rId6" xr:uid="{A4CE1694-91E7-453B-981E-2C795B08BDB0}"/>
+    <hyperlink ref="T5" r:id="rId7" xr:uid="{1D2555EE-CED0-4CD9-9E68-36AA5010E3B0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+</worksheet>
 </file>
</xml_diff>